<commit_message>
add the function to exclude either chi or eng string
</commit_message>
<xml_diff>
--- a/Extract.xlsx
+++ b/Extract.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MEI WAN BUILDING, 4 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊4號 美雲樓 (大廈)</t>
+          <t>LAI CHUN BUILDING, 16 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊16號 麗珍樓 (大廈)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -493,34 +493,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>UDR00399/NT/21/AEF/VH(5OJ118)</t>
+          <t>DR00058/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>大埔鄉事會坊4號美雲樓四樓B室</t>
+          <t>大埔娜事會坊16號麗珍樓三樓B室</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022年11月29日</t>
+          <t>2022年6月21日</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>第24條命令（只涉及渠務）</t>
+          <t>第28條渠務修葺令／勘測令</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>EB/9159/69/2/E03(SDI-AEF)</t>
+          <t>EB/9336/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MEI WAN BUILDING, 4 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊4號 美雲樓 (大廈)</t>
+          <t>LAI CHUN BUILDING, 16 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊16號 麗珍樓 (大廈)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -535,34 +535,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>UDR00400/NT/21/AEF/VH(5OJ118)</t>
+          <t>DR00060/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>大埔鄉事會坊4號美雲樓五樓B室</t>
+          <t>大埔娜事會坊16號麗珍樓四樓C室</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022年11月29日</t>
+          <t>2022年6月21日</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>第24條命令（只涉及渠務）</t>
+          <t>第28條渠務修葺令／勘測令</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>EB/9159/69/2/E03(SDI-AEF)</t>
+          <t>EB/9336/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MEI WAN BUILDING, 4 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊4號 美雲樓 (大廈)</t>
+          <t>LAI CHUN BUILDING, 16 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊16號 麗珍樓 (大廈)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -577,39 +577,39 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>UDR00401/NT/21/AEF/VH(5OJ118)</t>
+          <t>DR00059/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>大埔鄉事會坊4號美雲樓六樓B室及天台</t>
+          <t>大埔娜事會坊16號麗珍樓六樓C及天台</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2022年11月29日</t>
+          <t>2022年6月21日</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>第24條命令（只涉及渠務）</t>
+          <t>第28條渠務修葺令／勘測令</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>EB/9159/69/2/E03(SDI-AEF)</t>
+          <t>EB/9336/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MEI WAN BUILDING, 6 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊6號 美雲樓 (大廈)</t>
+          <t>KAM MING BUILDING, 18 - 20 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊18 - 20號 (大廈)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>樓宇公用部份</t>
+          <t>個別單位</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -619,34 +619,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>DR00406/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00227/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>大埔鄉事會坊4/6號美雲樓</t>
+          <t>"大埔 鄉事會坊20號 金明樓 四樓 A室"</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022年11月29日</t>
+          <t>2022年10月25日</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>第28條渠務修葺令／勘測令</t>
+          <t>第24條命令（只涉及渠務）</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>EB/9159/69/1/E03(SDI-AEF)</t>
+          <t>EB/9009/71/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MEI WAN BUILDING, 6 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊6號 美雲樓 (大廈)</t>
+          <t>KAM MING BUILDING, 18 - 20 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊18 - 20號 (大廈)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -661,17 +661,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>UDR00404/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00228/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>大埔鄉事會坊6號美雲樓五樓D室</t>
+          <t>大埔 鄉事會坊20號 金明樓 五樓 A室</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2022年11月29日</t>
+          <t>2022年10月25日</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -681,14 +681,14 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>EB/9159/69/1/E03(SDI-AEF)</t>
+          <t>EB/9009/71/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MEI WAN BUILDING, 6 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊6號 美雲樓 (大廈)</t>
+          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -698,22 +698,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>未獲遵從</t>
+          <t>已獲遵從</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>UDR00403/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00751/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>大埔鄉事會坊6號美雲樓六樓D室及天台</t>
+          <t>大埔 大榮里40號美發大廈四樓 F室</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022年11月29日</t>
+          <t>2022年12月9日</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -723,14 +723,14 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>EB/9159/69/1/E03(SDI-AEF)</t>
+          <t>EB/9251/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LAI CHUN BUILDING, 16 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊16號 麗珍樓 (大廈)</t>
+          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -740,39 +740,39 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>未獲遵從</t>
+          <t>已獲遵從</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>DR00058/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00752/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>大埔娜事會坊16號麗珍樓三樓B室</t>
+          <t>大埔 大榮里40號美發大廈五樓 F室</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022年6月21日</t>
+          <t>2022年12月9日</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>第28條渠務修葺令／勘測令</t>
+          <t>第24條命令（只涉及渠務）</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>EB/9336/70/E03(SDI-AEF)</t>
+          <t>EB/9251/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LAI CHUN BUILDING, 16 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊16號 麗珍樓 (大廈)</t>
+          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -782,39 +782,39 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>未獲遵從</t>
+          <t>已獲遵從</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>DR00060/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00753/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>大埔娜事會坊16號麗珍樓四樓C室</t>
+          <t>大埔 大榮里40號美發大廈七樓 F室</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022年6月21日</t>
+          <t>2022年12月9日</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>第28條渠務修葺令／勘測令</t>
+          <t>第24條命令（只涉及渠務）</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>EB/9336/70/E03(SDI-AEF)</t>
+          <t>EB/9251/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LAI CHUN BUILDING, 16 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊16號 麗珍樓 (大廈)</t>
+          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -824,39 +824,39 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>未獲遵從</t>
+          <t>已獲遵從</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>DR00059/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00754/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>大埔娜事會坊16號麗珍樓六樓C及天台</t>
+          <t>大埔 大榮里40號 美發大廈 十二樓 D室</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2022年6月21日</t>
+          <t>2022年12月9日</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>第28條渠務修葺令／勘測令</t>
+          <t>第24條命令（只涉及渠務）</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>EB/9336/70/E03(SDI-AEF)</t>
+          <t>EB/9251/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KAM MING BUILDING, 18 - 20 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊18 - 20號 (大廈)</t>
+          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -866,22 +866,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>未獲遵從</t>
+          <t>已獲遵從</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>UDR00227/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00755/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>"大埔 鄉事會坊20號 金明樓 四樓 A室"</t>
+          <t>大埔 大榮里40號 美發大廈 十二樓 F室</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2022年10月25日</t>
+          <t>2022年12月9日</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -891,14 +891,14 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>EB/9009/71/E03(SDI-AEF)</t>
+          <t>EB/9251/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KAM MING BUILDING, 18 - 20 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊18 - 20號 (大廈)</t>
+          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -908,22 +908,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>未獲遵從</t>
+          <t>已獲遵從</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>UDR00228/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00756/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>大埔 鄉事會坊20號 金明樓 五樓 A室</t>
+          <t>大埔 大榮里40號美發大廈十四樓 D室</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022年10月25日</t>
+          <t>2022年12月9日</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>EB/9009/71/E03(SDI-AEF)</t>
+          <t>EB/9251/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
@@ -955,12 +955,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>UDR00751/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00757/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>大埔 大榮里40號美發大廈四樓 F室</t>
+          <t>大埔 大榮里40號美發大廈十四樓 E室</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -982,7 +982,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
+          <t>YUK WAH COURT, 35 - 37 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊35 - 37號 玉華閣 (大廈)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -992,39 +992,39 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>已獲遵從</t>
+          <t>未獲遵從</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>UDR00752/NT/21/AEF/VH(5OJ118)</t>
+          <t>DR00034/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>大埔 大榮里40號美發大廈五樓 F室</t>
+          <t>Flat A on 2/F Yuk Wah Court Nos. 17 &amp; 19 Tai Kwong Lane Nos. 35 &amp; 37 Heung Sze Wui Square Tai Po, New Territories</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022年12月9日</t>
+          <t>2022年5月18日</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>第24條命令（只涉及渠務）</t>
+          <t>第28條渠務修葺令／勘測令</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>EB/9251/70/E03(SDI-AEF)</t>
+          <t>EB/9183/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
+          <t>YUK WAH COURT, 35 - 37 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊35 - 37號 玉華閣 (大廈)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1034,39 +1034,39 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>已獲遵從</t>
+          <t>未獲遵從</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>UDR00753/NT/21/AEF/VH(5OJ118)</t>
+          <t>DR00035/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>大埔 大榮里40號美發大廈七樓 F室</t>
+          <t>Flat A on 3/F Yuk Wah Court Nos. 17 &amp; 19 Tai Kwong Lane Nos. 35 &amp; 37 Heung Sze Wui Square Tai Po, New Territories</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022年12月9日</t>
+          <t>2022年5月18日</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>第24條命令（只涉及渠務）</t>
+          <t>第28條渠務修葺令／勘測令</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>EB/9251/70/E03(SDI-AEF)</t>
+          <t>EB/9183/70/E03(SDI-AEF)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
+          <t>PING ON BUILDING, 43 - 47 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊43 - 47號 平安樓 (大廈)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>UDR00754/NT/21/AEF/VH(5OJ118)</t>
+          <t>UDR00088/NT/21/AEF/VH(5OJ118)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>大埔 大榮里40號 美發大廈 十二樓 D室</t>
+          <t>大埔鄉事會坊47號平安樓五樓C室</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022年12月9日</t>
+          <t>2022年9月2日</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1100,258 +1100,6 @@
         </is>
       </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>EB/9251/70/E03(SDI-AEF)</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>個別單位</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>已獲遵從</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>UDR00755/NT/21/AEF/VH(5OJ118)</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>大埔 大榮里40號 美發大廈 十二樓 F室</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2022年12月9日</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>第24條命令（只涉及渠務）</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>EB/9251/70/E03(SDI-AEF)</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>個別單位</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>已獲遵從</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>UDR00756/NT/21/AEF/VH(5OJ118)</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>大埔 大榮里40號美發大廈十四樓 D室</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2022年12月9日</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>第24條命令（只涉及渠務）</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>EB/9251/70/E03(SDI-AEF)</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>MEI FAT BUILDING, 25 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊25號 美發大廈 (大廈)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>個別單位</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>已獲遵從</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>UDR00757/NT/21/AEF/VH(5OJ118)</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>大埔 大榮里40號美發大廈十四樓 E室</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2022年12月9日</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>第24條命令（只涉及渠務）</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>EB/9251/70/E03(SDI-AEF)</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>YUK WAH COURT, 35 - 37 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊35 - 37號 玉華閣 (大廈)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>個別單位</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>未獲遵從</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>DR00034/NT/21/AEF/VH(5OJ118)</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Flat A on 2/F Yuk Wah Court Nos. 17 &amp; 19 Tai Kwong Lane Nos. 35 &amp; 37 Heung Sze Wui Square Tai Po, New Territories</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2022年5月18日</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>第28條渠務修葺令／勘測令</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>EB/9183/70/E03(SDI-AEF)</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>YUK WAH COURT, 35 - 37 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊35 - 37號 玉華閣 (大廈)</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>個別單位</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>未獲遵從</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>DR00035/NT/21/AEF/VH(5OJ118)</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Flat A on 3/F Yuk Wah Court Nos. 17 &amp; 19 Tai Kwong Lane Nos. 35 &amp; 37 Heung Sze Wui Square Tai Po, New Territories</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2022年5月18日</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>第28條渠務修葺令／勘測令</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>EB/9183/70/E03(SDI-AEF)</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>PING ON BUILDING, 43 - 47 HEUNG SZE WUI SQUARE (Tower Block) 大埔 鄉事會坊43 - 47號 平安樓 (大廈)</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>個別單位</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>已獲遵從</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>UDR00088/NT/21/AEF/VH(5OJ118)</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>大埔鄉事會坊47號平安樓五樓C室</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2022年9月2日</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>第24條命令（只涉及渠務）</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
         <is>
           <t>EB/9045/70/1/E03(SDI-AEF)</t>
         </is>

</xml_diff>